<commit_message>
upload part of 1-300 easy
</commit_message>
<xml_diff>
--- a/LeetCode1-300/LeetCode1-300.xlsx
+++ b/LeetCode1-300/LeetCode1-300.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\leetcode\LeetCode 101：和你一起你轻松刷题\LeetCode1-300\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390F301E-6AE0-4ADD-AED4-DE5450578C2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15451EF8-48DD-4488-981E-7D4A983FDE58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1290" windowWidth="29040" windowHeight="15840" xr2:uid="{4A132E47-3C93-46B5-A3C4-5EBA1D570D7E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
   <si>
     <t>Array, Hash Table, N-Sum</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -322,17 +322,10 @@
     <t>53. Maximum Subarray</t>
   </si>
   <si>
-    <t>最大连续子数组之和</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1. Two Sum</t>
-  </si>
-  <si>
     <t>7. Reverse Integer</t>
   </si>
   <si>
@@ -382,20 +375,12 @@
     <t>69. Sqrt(x)</t>
   </si>
   <si>
-    <t>求给定值的正整数平方根</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>69. Sqrt(x).md</t>
   </si>
   <si>
     <t>70. Climbing Stairs</t>
   </si>
   <si>
-    <t>爬楼梯一步或两步，有多少不同的方式爬到楼顶</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>70. Climbing Stairs.md</t>
   </si>
   <si>
@@ -403,10 +388,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>判断树相同对称平衡，DFS和BFS遍历树</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Tree</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -421,12 +402,348 @@
     <t>118. Pascal's Triangle</t>
   </si>
   <si>
+    <t>easy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>118. Pascal's Triangle.md</t>
+  </si>
+  <si>
+    <t>DP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">121/122 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>股票买卖</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>121. Best Time to Buy and Sell Stock.md</t>
+  </si>
+  <si>
+    <t>125. Valid Palindrome</t>
+  </si>
+  <si>
+    <t>easy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>136. Single Number</t>
+  </si>
+  <si>
+    <t>125. Valid Palindrome.md</t>
+  </si>
+  <si>
+    <t>136. Single Number.md</t>
+  </si>
+  <si>
+    <t>HashSet, Bit Manipulation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>快慢指针，相遇后重置</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>slow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，再一起走直到相遇</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>155. Min Stack</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>设计一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Stack</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>可以返回最小元素</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Design, Stack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>stack</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>存元素，一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>stack</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>顶存最小值</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">141/142/160 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>链表环，两个链表相交点</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/167. Two Sum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最大连续子数组之和</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>求给定值的正整数平方根</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>爬楼梯一步或两步，有多少不同的方式爬到楼顶</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>判断树相同对称平衡，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DFS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>BFS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>遍历树</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>买卖股票，在数组中找到最大差值</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>判断字符串是否为回文</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数组中只有一个数没有重复数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>判断链表是否有环和环的入口，找两个相交的点</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="14"/>
         <color rgb="FF263238"/>
         <rFont val="宋体"/>
         <family val="2"/>
@@ -436,16 +753,16 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="14"/>
         <color rgb="FF263238"/>
-        <rFont val="Segoe UI"/>
+        <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
       <t>N</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="14"/>
         <color rgb="FF263238"/>
         <rFont val="宋体"/>
         <family val="2"/>
@@ -455,16 +772,16 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="14"/>
         <color rgb="FF263238"/>
-        <rFont val="Segoe UI"/>
+        <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">Pascal's </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="14"/>
         <color rgb="FF263238"/>
         <rFont val="宋体"/>
         <family val="2"/>
@@ -474,16 +791,16 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="14"/>
         <color rgb="FF263238"/>
-        <rFont val="Segoe UI"/>
+        <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
       <t>N</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="14"/>
         <color rgb="FF263238"/>
         <rFont val="宋体"/>
         <family val="2"/>
@@ -494,46 +811,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>easy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>118. Pascal's Triangle.md</t>
-  </si>
-  <si>
-    <t>DP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>买卖股票，在数组中找到最大差值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">121/122 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>股票买卖</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>121. Best Time to Buy and Sell Stock.md</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>给定一个正整数返回</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Excel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>式的字符串</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Math</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>168/171. Excel Sheet Column Title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,28 +923,21 @@
     </font>
     <font>
       <b/>
-      <sz val="22"/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF263238"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF263238"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="14"/>
-      <color theme="1"/>
+      <color rgb="FF263238"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF263238"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
@@ -653,11 +968,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -675,12 +987,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -690,20 +996,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1023,364 +1326,434 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="52.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="29.75" style="2" customWidth="1"/>
-    <col min="5" max="5" width="49.875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.25" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="46.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="50.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="E21" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
+      <c r="D23" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
+      <c r="A24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
+      <c r="A25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
+      <c r="A26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
+      <c r="A27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
+      <c r="A28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
+      <c r="A29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
+      <c r="A30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
+      <c r="A31" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E57">
@@ -1400,7 +1773,7 @@
     <hyperlink ref="E9" r:id="rId10" xr:uid="{F5005A9B-D66B-4183-8EFA-E1899C090F00}"/>
     <hyperlink ref="E10" r:id="rId11" xr:uid="{8591D6D4-BC7A-404B-A218-774B6B2565A6}"/>
     <hyperlink ref="A11" r:id="rId12" xr:uid="{5718B284-793A-4B58-B16B-5EA269A10710}"/>
-    <hyperlink ref="A2" r:id="rId13" xr:uid="{66ADA23A-EEC0-417E-BB29-F5E892238E60}"/>
+    <hyperlink ref="A2" r:id="rId13" display="1. Two Sum" xr:uid="{66ADA23A-EEC0-417E-BB29-F5E892238E60}"/>
     <hyperlink ref="A12" r:id="rId14" xr:uid="{5F9565F1-3463-4DFD-891E-03F1F7653C8D}"/>
     <hyperlink ref="A13" r:id="rId15" xr:uid="{0E143C9D-001F-4457-A8C9-322FE4981BD2}"/>
     <hyperlink ref="A3" r:id="rId16" xr:uid="{7977C004-3D02-4E99-8629-3F1AD8CAD91A}"/>
@@ -1421,8 +1794,14 @@
     <hyperlink ref="A17" r:id="rId31" xr:uid="{963B3F81-4518-4D74-82B5-2A5F6CE02400}"/>
     <hyperlink ref="E17" r:id="rId32" xr:uid="{69DA9854-D1C2-4CCA-BFC3-4C642FFFFAA7}"/>
     <hyperlink ref="E18" r:id="rId33" xr:uid="{D15692AE-2EE6-4D7A-83EB-4E57C68F6619}"/>
+    <hyperlink ref="A19" r:id="rId34" xr:uid="{1FF2D0DF-2ECB-4993-88CC-2C2DA53C5058}"/>
+    <hyperlink ref="A20" r:id="rId35" xr:uid="{9698D476-38CB-4BF8-8E4E-77771B22FFB7}"/>
+    <hyperlink ref="E19" r:id="rId36" xr:uid="{03B2B8EC-6E5C-4247-A5DB-2C452CE09669}"/>
+    <hyperlink ref="E20" r:id="rId37" xr:uid="{473A5174-537B-49AF-8BFE-87FF0E6432FE}"/>
+    <hyperlink ref="A22" r:id="rId38" xr:uid="{FCD906F0-8012-479E-B9DA-00BF6CB23622}"/>
+    <hyperlink ref="A23" r:id="rId39" display="168. Excel Sheet Column Title" xr:uid="{BA69FBA0-E204-4A3B-9888-D9B46E29AA9C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>